<commit_message>
download any number of guides
</commit_message>
<xml_diff>
--- a/new_lethality.xlsx
+++ b/new_lethality.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="28">
   <si>
     <t>index</t>
   </si>
@@ -47,15 +47,6 @@
   </si>
   <si>
     <t>genes_2,3_synth</t>
-  </si>
-  <si>
-    <t>YIL149C</t>
-  </si>
-  <si>
-    <t>YLR309C</t>
-  </si>
-  <si>
-    <t>YJL016W</t>
   </si>
   <si>
     <t>YGL263W</t>
@@ -464,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -507,382 +498,268 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>2369</v>
+        <v>2389</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F2">
-        <v>1.039167804658413</v>
+        <v>1.034627103447914</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>2359</v>
+        <v>2422</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F3">
-        <v>1.036482501685619</v>
+        <v>1.032986598968506</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>2425</v>
+        <v>2374</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4">
-        <v>1.036174698114395</v>
+        <v>1.031123504281044</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>2389</v>
+        <v>2429</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5">
-        <v>1.034627103447914</v>
+        <v>1.02994580489397</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>2422</v>
+        <v>2376</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6">
-        <v>1.032986598968506</v>
+        <v>1.028615909814835</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>2374</v>
+        <v>2324</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
       <c r="F7">
-        <v>1.031123504281044</v>
+        <v>1.028593597054482</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>2429</v>
+        <v>2321</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8">
-        <v>1.02994580489397</v>
+        <v>1.028387402355671</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>2376</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9">
-        <v>1.028615909814835</v>
-      </c>
-      <c r="G9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>2324</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10">
-        <v>1.028593597054482</v>
-      </c>
-      <c r="G10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>2321</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11">
-        <v>1.028387402355671</v>
-      </c>
-      <c r="G11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>